<commit_message>
Filtro xml nomina funcional y acumulado solo excel sin formato
</commit_message>
<xml_diff>
--- a/application/controllers/acumulados/RFCEMP2017.xlsx
+++ b/application/controllers/acumulados/RFCEMP2017.xlsx
@@ -2893,11 +2893,11 @@
   <dimension ref="A1:BK455"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="BJ120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="BJ454" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I31" sqref="I31"/>
       <selection pane="topRight" activeCell="I31" sqref="I31"/>
       <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:A128"/>
+      <selection pane="bottomRight" activeCell="B465" sqref="B465:C474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>